<commit_message>
added collision count to xlsx
</commit_message>
<xml_diff>
--- a/src/hash_analysis.xlsx
+++ b/src/hash_analysis.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="75">
   <si>
     <t xml:space="preserve">Bit Ratios by Filetype</t>
   </si>
@@ -187,6 +187,12 @@
     <t xml:space="preserve">This graph shows the average ratio of 1s and 0s in columns across the 5 file types, but the ratios have been sorted from lowest to highest.
 Ratios close to 0.5 are best, ratios near 0 or 1 indicate significant skew. 
 We would expect more random types of input, like random or shak, to do better than less random times, like a, ones, or zero. In fact, we see that the ratios for random hover around 0.5, while the ratios for zero hover near zero for 8 bits, and hover near 1 for the remaining 24 bits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filetype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collisions (out of 10000)</t>
   </si>
   <si>
     <t xml:space="preserve">filetype_a</t>
@@ -434,7 +440,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -859,11 +865,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="1835296"/>
-        <c:axId val="59303746"/>
+        <c:axId val="42189985"/>
+        <c:axId val="84666761"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1835296"/>
+        <c:axId val="42189985"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,7 +925,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59303746"/>
+        <c:crossAx val="84666761"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -927,7 +933,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59303746"/>
+        <c:axId val="84666761"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +998,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835296"/>
+        <c:crossAx val="42189985"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1040,7 +1046,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1851,11 +1857,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="92159643"/>
-        <c:axId val="10905527"/>
+        <c:axId val="71048084"/>
+        <c:axId val="36982169"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92159643"/>
+        <c:axId val="71048084"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1911,7 +1917,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10905527"/>
+        <c:crossAx val="36982169"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1919,7 +1925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10905527"/>
+        <c:axId val="36982169"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1984,7 +1990,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92159643"/>
+        <c:crossAx val="71048084"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2032,7 +2038,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2843,11 +2849,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="35473936"/>
-        <c:axId val="45017223"/>
+        <c:axId val="24504856"/>
+        <c:axId val="94641729"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="35473936"/>
+        <c:axId val="24504856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2903,7 +2909,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45017223"/>
+        <c:crossAx val="94641729"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2911,7 +2917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45017223"/>
+        <c:axId val="94641729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2976,7 +2982,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35473936"/>
+        <c:crossAx val="24504856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3024,7 +3030,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3870,11 +3876,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="20181896"/>
-        <c:axId val="28771764"/>
+        <c:axId val="26716118"/>
+        <c:axId val="42512048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="20181896"/>
+        <c:axId val="26716118"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3930,7 +3936,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28771764"/>
+        <c:crossAx val="42512048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3938,7 +3944,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28771764"/>
+        <c:axId val="42512048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4003,7 +4009,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20181896"/>
+        <c:crossAx val="26716118"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4051,6 +4057,303 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Collisions per File Type</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphs!$C$114</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>collisions (out of 10000)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>graphs!$B$115:$B$119</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>zero</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>random</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>shak</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>graphs!$C$115:$C$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2917</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="53154419"/>
+        <c:axId val="26500556"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="53154419"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>File Type</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="26500556"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="26500556"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Collisions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53154419"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -4061,8 +4364,8 @@
       <xdr:rowOff>103320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>26640</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>181440</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
@@ -4091,8 +4394,8 @@
       <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>21240</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>176040</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
@@ -4122,7 +4425,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>50040</xdr:colOff>
+      <xdr:colOff>50400</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
@@ -4132,7 +4435,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6480000" y="6502680"/>
+        <a:off x="6681960" y="6502680"/>
         <a:ext cx="5757120" cy="3241800"/>
       </xdr:xfrm>
       <a:graphic>
@@ -4151,8 +4454,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>109080</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>264240</xdr:colOff>
       <xdr:row>111</xdr:row>
       <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
@@ -4173,6 +4476,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209880</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>76680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4033800" y="18292680"/>
+        <a:ext cx="5768640" cy="3241800"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4181,16 +4514,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AH103"/>
+  <dimension ref="A2:AH119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE91" activeCellId="0" sqref="AE91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB117" activeCellId="0" sqref="AB117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="3" style="0" width="5.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="4" style="0" width="5.06"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7942,6 +8276,59 @@
       <c r="W103" s="2"/>
       <c r="X103" s="2"/>
       <c r="Y103" s="2"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <f aca="false">data!B8</f>
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <f aca="false">data!B26</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <f aca="false">data!B44</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <f aca="false">data!B62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <f aca="false">data!B80</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7969,20 +8356,20 @@
   </sheetPr>
   <dimension ref="A1:AG89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B80" activeCellId="0" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>32</v>
@@ -7990,7 +8377,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2917</v>
@@ -7998,13 +8385,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.71875</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.0494105884401309</v>
@@ -8012,13 +8399,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.71875</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0.329239179776648</v>
@@ -8026,7 +8413,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -8127,7 +8514,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -8228,7 +8615,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2917</v>
@@ -8236,12 +8623,12 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>32</v>
@@ -8249,7 +8636,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>10000</v>
@@ -8257,13 +8644,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0</v>
@@ -8271,13 +8658,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0</v>
@@ -8285,7 +8672,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.96875</v>
@@ -8386,7 +8773,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.96875</v>
@@ -8487,7 +8874,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -8495,12 +8882,12 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>32</v>
@@ -8508,7 +8895,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>10000</v>
@@ -8516,13 +8903,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0.146575492494482</v>
@@ -8530,13 +8917,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -8544,7 +8931,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.5</v>
@@ -8645,7 +9032,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0.5</v>
@@ -8746,7 +9133,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>10000</v>
@@ -8754,12 +9141,12 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>32</v>
@@ -8767,7 +9154,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>10000</v>
@@ -8775,13 +9162,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
@@ -8789,13 +9176,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>0</v>
@@ -8803,7 +9190,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0.96875</v>
@@ -8904,7 +9291,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0.96875</v>
@@ -9005,7 +9392,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0</v>
@@ -9013,12 +9400,12 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>32</v>
@@ -9026,7 +9413,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>10000</v>
@@ -9034,13 +9421,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0.75</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0</v>
@@ -9048,13 +9435,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0.75</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>0.433012701892219</v>
@@ -9062,7 +9449,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
@@ -9163,7 +9550,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0</v>
@@ -9264,7 +9651,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>10000</v>
@@ -9272,12 +9659,12 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>32</v>
@@ -9285,7 +9672,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>10000</v>
@@ -9293,13 +9680,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>0</v>
@@ -9307,13 +9694,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>0</v>
@@ -9321,7 +9708,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0.96875</v>
@@ -9422,7 +9809,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0.96875</v>
@@ -9523,7 +9910,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -9531,12 +9918,12 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>32</v>
@@ -9544,7 +9931,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>10000</v>
@@ -9552,13 +9939,13 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0.501571875</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>0.0887036075378807</v>
@@ -9566,13 +9953,13 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>0.501571875</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>0.00476577868604648</v>
@@ -9580,7 +9967,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0.4903</v>
@@ -9681,7 +10068,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0.4903</v>
@@ -9782,7 +10169,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0</v>
@@ -9790,12 +10177,12 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>32</v>
@@ -9803,7 +10190,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>10000</v>
@@ -9811,13 +10198,13 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>0</v>
@@ -9825,13 +10212,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>0</v>
@@ -9839,7 +10226,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0.96875</v>
@@ -9940,7 +10327,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0.96875</v>
@@ -10041,7 +10428,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -10049,12 +10436,12 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>32</v>
@@ -10062,7 +10449,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>10000</v>
@@ -10070,13 +10457,13 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>0.5623</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0.0829142007589774</v>
@@ -10084,13 +10471,13 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0.5623</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>0.165529083547273</v>
@@ -10098,7 +10485,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -10199,7 +10586,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>0.4874</v>
@@ -10300,7 +10687,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>0</v>
@@ -10308,12 +10695,12 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>32</v>
@@ -10321,7 +10708,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>10000</v>
@@ -10329,13 +10716,13 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>0</v>
@@ -10343,13 +10730,13 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>0.96875</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>0</v>
@@ -10357,7 +10744,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>0.96875</v>
@@ -10458,7 +10845,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>0.96875</v>
@@ -10559,7 +10946,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>0</v>

</xml_diff>